<commit_message>
addition of data sources for finance
</commit_message>
<xml_diff>
--- a/Notes_and_Guides/IRS_Data_Sources.xlsx
+++ b/Notes_and_Guides/IRS_Data_Sources.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="74">
   <si>
     <t>Subchapter C corporations</t>
   </si>
@@ -169,13 +169,90 @@
   </si>
   <si>
     <t>2011sb3</t>
+  </si>
+  <si>
+    <t>Variable Name</t>
+  </si>
+  <si>
+    <t>INTRST_PD</t>
+  </si>
+  <si>
+    <t>DPRCBL_ASSTS</t>
+  </si>
+  <si>
+    <t>ACCUM_DPR</t>
+  </si>
+  <si>
+    <t>LAND</t>
+  </si>
+  <si>
+    <t>INVNTRY</t>
+  </si>
+  <si>
+    <t>CAP_STCK</t>
+  </si>
+  <si>
+    <t>PD_CAP_SRPLS</t>
+  </si>
+  <si>
+    <t>RTND_ERNGS_APPR+COMP_RTND_ERNGS_UNAPPR</t>
+  </si>
+  <si>
+    <t>CST_TRSRY_STCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Depreciation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Inventory, beginning of year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Depreciable assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Less:  Accumulated depreciation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Land</t>
+  </si>
+  <si>
+    <t>Income (loss) allocated to partners by type of
+   partner [1]:</t>
+  </si>
+  <si>
+    <t>Interest Paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Interest paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Partners capital accounts </t>
+  </si>
+  <si>
+    <t>Partners Capital Accounts</t>
+  </si>
+  <si>
+    <t>Interest paid deduction [1,3]</t>
+  </si>
+  <si>
+    <t>Depreciation deduction [1,2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Inventory, beginning of year</t>
+  </si>
+  <si>
+    <t>11sp01is</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0&quot;  &quot;;\-#,##0&quot;  &quot;;&quot;0  &quot;;@&quot; &quot;"/>
+    <numFmt numFmtId="165" formatCode="@*."/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -199,6 +276,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Helv"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -214,7 +319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -222,8 +327,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="55"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="55"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -311,12 +464,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="87"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="94" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="107" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -360,6 +544,23 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -403,7 +604,11 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_Table 3" xfId="93"/>
+    <cellStyle name="Normal_Table 5 final" xfId="94"/>
+    <cellStyle name="style_stub_lines" xfId="107"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -732,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:A51"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -744,15 +949,15 @@
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -763,19 +968,22 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -785,20 +993,23 @@
       <c r="C3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
         <v>48</v>
       </c>
-      <c r="E3">
-        <v>2011</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>2011</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -808,17 +1019,20 @@
       <c r="C4" t="s">
         <v>47</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
         <v>48</v>
       </c>
-      <c r="E4">
-        <v>2011</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="F4">
+        <v>2011</v>
+      </c>
+      <c r="I4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -828,14 +1042,17 @@
       <c r="C5" t="s">
         <v>47</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
         <v>48</v>
       </c>
-      <c r="E5">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="F5">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -845,14 +1062,17 @@
       <c r="C6" t="s">
         <v>47</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
         <v>48</v>
       </c>
-      <c r="E6">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="F6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -862,14 +1082,17 @@
       <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
         <v>48</v>
       </c>
-      <c r="E7">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="F7">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -879,14 +1102,17 @@
       <c r="C8" t="s">
         <v>47</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
         <v>48</v>
       </c>
-      <c r="E8">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="F8">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -896,14 +1122,17 @@
       <c r="C9" t="s">
         <v>47</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
         <v>48</v>
       </c>
-      <c r="E9">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="F9">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -913,14 +1142,17 @@
       <c r="C10" t="s">
         <v>47</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
         <v>48</v>
       </c>
-      <c r="E10">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="F10">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -930,19 +1162,22 @@
       <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
         <v>48</v>
       </c>
-      <c r="E11">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="F11">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -953,16 +1188,19 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
         <v>4</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>20</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -972,17 +1210,20 @@
       <c r="C15" t="s">
         <v>47</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
         <v>49</v>
       </c>
-      <c r="E15">
-        <v>2011</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="F15">
+        <v>2011</v>
+      </c>
+      <c r="G15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -992,14 +1233,17 @@
       <c r="C16" t="s">
         <v>47</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
         <v>49</v>
       </c>
-      <c r="E16">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="F16">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1009,14 +1253,17 @@
       <c r="C17" t="s">
         <v>47</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
         <v>49</v>
       </c>
-      <c r="E17">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="F17">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1026,14 +1273,17 @@
       <c r="C18" t="s">
         <v>47</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
         <v>49</v>
       </c>
-      <c r="E18">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="F18">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1043,14 +1293,17 @@
       <c r="C19" t="s">
         <v>47</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" t="s">
         <v>49</v>
       </c>
-      <c r="E19">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="F19">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1060,14 +1313,17 @@
       <c r="C20" t="s">
         <v>47</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
         <v>49</v>
       </c>
-      <c r="E20">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="F20">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1077,14 +1333,17 @@
       <c r="C21" t="s">
         <v>47</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" t="s">
         <v>49</v>
       </c>
-      <c r="E21">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="F21">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1094,14 +1353,17 @@
       <c r="C22" t="s">
         <v>47</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" t="s">
         <v>49</v>
       </c>
-      <c r="E22">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="F22">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1111,19 +1373,22 @@
       <c r="C23" t="s">
         <v>47</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
         <v>49</v>
       </c>
-      <c r="E23">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="F23">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1134,16 +1399,19 @@
         <v>3</v>
       </c>
       <c r="D26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" t="s">
         <v>4</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>20</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1154,16 +1422,19 @@
         <v>34</v>
       </c>
       <c r="D27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" t="s">
         <v>35</v>
       </c>
-      <c r="E27">
-        <v>2011</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="F27">
+        <v>2011</v>
+      </c>
+      <c r="G27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1173,290 +1444,268 @@
       <c r="C28" t="s">
         <v>34</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" t="s">
         <v>35</v>
       </c>
-      <c r="E28">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
+      <c r="F29">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
         <v>1</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" t="s">
         <v>2</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C34" t="s">
         <v>3</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" t="s">
         <v>4</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F34" t="s">
         <v>20</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
         <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32">
-        <v>67</v>
-      </c>
-      <c r="E32">
-        <v>2012</v>
-      </c>
-      <c r="F32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33">
-        <v>67</v>
-      </c>
-      <c r="E33">
-        <v>2012</v>
-      </c>
-      <c r="F33" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34">
-        <v>67</v>
-      </c>
-      <c r="E34">
-        <v>2012</v>
-      </c>
-      <c r="F34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
-        <v>42</v>
       </c>
       <c r="C35" t="s">
         <v>37</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>67</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>2012</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36">
+        <v>67</v>
+      </c>
+      <c r="F36">
+        <v>2012</v>
+      </c>
+      <c r="G36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37">
+        <v>67</v>
+      </c>
+      <c r="F37">
+        <v>2012</v>
+      </c>
+      <c r="G37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38">
+        <v>67</v>
+      </c>
+      <c r="F38">
+        <v>2012</v>
+      </c>
+      <c r="G38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
         <v>43</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G40" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="s">
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
         <v>1</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>2</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C41" t="s">
         <v>3</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D41" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" t="s">
         <v>4</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F41" t="s">
         <v>20</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G41" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" t="s">
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
         <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39">
-        <v>67</v>
-      </c>
-      <c r="E39">
-        <v>2012</v>
-      </c>
-      <c r="F39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40">
-        <v>67</v>
-      </c>
-      <c r="E40">
-        <v>2012</v>
-      </c>
-      <c r="F40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41">
-        <v>67</v>
-      </c>
-      <c r="E41">
-        <v>2012</v>
-      </c>
-      <c r="F41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
-        <v>42</v>
       </c>
       <c r="C42" t="s">
         <v>37</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>67</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>2012</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="E43">
+        <v>67</v>
+      </c>
+      <c r="F43">
+        <v>2012</v>
+      </c>
+      <c r="G43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44">
+        <v>67</v>
+      </c>
+      <c r="F44">
+        <v>2012</v>
+      </c>
+      <c r="G44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45">
+        <v>67</v>
+      </c>
+      <c r="F45">
+        <v>2012</v>
+      </c>
+      <c r="G45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
         <v>1</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B49" t="s">
         <v>2</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C49" t="s">
         <v>3</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D49" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" t="s">
         <v>4</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F49" t="s">
         <v>20</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G49" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47" t="s">
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
         <v>23</v>
-      </c>
-      <c r="B47" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" t="s">
-        <v>28</v>
-      </c>
-      <c r="E47">
-        <v>2012</v>
-      </c>
-      <c r="F47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" t="s">
-        <v>31</v>
-      </c>
-      <c r="D48" t="s">
-        <v>28</v>
-      </c>
-      <c r="E48">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" t="s">
-        <v>19</v>
-      </c>
-      <c r="C49" t="s">
-        <v>31</v>
-      </c>
-      <c r="D49" t="s">
-        <v>29</v>
-      </c>
-      <c r="E49">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" t="s">
-        <v>6</v>
       </c>
       <c r="B50" t="s">
         <v>19</v>
@@ -1464,16 +1713,22 @@
       <c r="C50" t="s">
         <v>31</v>
       </c>
-      <c r="D50" t="s">
-        <v>29</v>
-      </c>
-      <c r="E50">
+      <c r="D50" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" t="s">
+        <v>28</v>
+      </c>
+      <c r="F50">
         <v>2012</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="G50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B51" t="s">
         <v>19</v>
@@ -1481,31 +1736,140 @@
       <c r="C51" t="s">
         <v>31</v>
       </c>
-      <c r="D51" t="s">
-        <v>29</v>
-      </c>
-      <c r="E51">
+      <c r="D51" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E51" t="s">
+        <v>28</v>
+      </c>
+      <c r="F51">
         <v>2012</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C52" t="s">
         <v>31</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E52" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" t="s">
+        <v>31</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E53" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" t="s">
+        <v>29</v>
+      </c>
+      <c r="F54">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15" customHeight="1">
+      <c r="A55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E55" t="s">
         <v>30</v>
       </c>
-      <c r="E52">
+      <c r="F55">
         <v>2012</v>
       </c>
     </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" t="s">
+        <v>31</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E57" t="s">
+        <v>29</v>
+      </c>
+      <c r="F57">
+        <v>2012</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>